<commit_message>
data fetching is fassst
</commit_message>
<xml_diff>
--- a/utils/yahoofinance/EDV_yahoofin_historical_data.xlsx
+++ b/utils/yahoofinance/EDV_yahoofin_historical_data.xlsx
@@ -539,7 +539,7 @@
         <v>86.989998</v>
       </c>
       <c r="F4" t="n">
-        <v>83.820297</v>
+        <v>83.820305</v>
       </c>
       <c r="G4" t="n">
         <v>383400</v>
@@ -639,7 +639,7 @@
         <v>89.5</v>
       </c>
       <c r="F8" t="n">
-        <v>86.23885300000001</v>
+        <v>86.238846</v>
       </c>
       <c r="G8" t="n">
         <v>158700</v>
@@ -739,7 +739,7 @@
         <v>92.83000199999999</v>
       </c>
       <c r="F12" t="n">
-        <v>89.447517</v>
+        <v>89.44750999999999</v>
       </c>
       <c r="G12" t="n">
         <v>334400</v>
@@ -814,7 +814,7 @@
         <v>89.5</v>
       </c>
       <c r="F15" t="n">
-        <v>86.23885300000001</v>
+        <v>86.238846</v>
       </c>
       <c r="G15" t="n">
         <v>250400</v>
@@ -839,7 +839,7 @@
         <v>91.239998</v>
       </c>
       <c r="F16" t="n">
-        <v>87.915443</v>
+        <v>87.915436</v>
       </c>
       <c r="G16" t="n">
         <v>161100</v>
@@ -1114,7 +1114,7 @@
         <v>89.970001</v>
       </c>
       <c r="F27" t="n">
-        <v>86.691727</v>
+        <v>86.69171900000001</v>
       </c>
       <c r="G27" t="n">
         <v>212600</v>
@@ -1264,7 +1264,7 @@
         <v>85.43000000000001</v>
       </c>
       <c r="F33" t="n">
-        <v>82.31714599999999</v>
+        <v>82.317154</v>
       </c>
       <c r="G33" t="n">
         <v>466900</v>
@@ -1339,7 +1339,7 @@
         <v>85.300003</v>
       </c>
       <c r="F36" t="n">
-        <v>82.19188699999999</v>
+        <v>82.191895</v>
       </c>
       <c r="G36" t="n">
         <v>115300</v>
@@ -1414,7 +1414,7 @@
         <v>85.160004</v>
       </c>
       <c r="F39" t="n">
-        <v>82.05699199999999</v>
+        <v>82.056984</v>
       </c>
       <c r="G39" t="n">
         <v>283500</v>
@@ -1614,7 +1614,7 @@
         <v>86.44000200000001</v>
       </c>
       <c r="F47" t="n">
-        <v>83.290344</v>
+        <v>83.290352</v>
       </c>
       <c r="G47" t="n">
         <v>143000</v>
@@ -1714,7 +1714,7 @@
         <v>90.449997</v>
       </c>
       <c r="F51" t="n">
-        <v>87.154228</v>
+        <v>87.154236</v>
       </c>
       <c r="G51" t="n">
         <v>341500</v>
@@ -1814,7 +1814,7 @@
         <v>89.30999799999999</v>
       </c>
       <c r="F55" t="n">
-        <v>86.05577099999999</v>
+        <v>86.055763</v>
       </c>
       <c r="G55" t="n">
         <v>845800</v>
@@ -1864,7 +1864,7 @@
         <v>89.910004</v>
       </c>
       <c r="F57" t="n">
-        <v>86.633911</v>
+        <v>86.633904</v>
       </c>
       <c r="G57" t="n">
         <v>884900</v>
@@ -1989,7 +1989,7 @@
         <v>88.610001</v>
       </c>
       <c r="F62" t="n">
-        <v>85.38127900000001</v>
+        <v>85.381271</v>
       </c>
       <c r="G62" t="n">
         <v>299600</v>
@@ -2014,7 +2014,7 @@
         <v>90.540001</v>
       </c>
       <c r="F63" t="n">
-        <v>87.24095199999999</v>
+        <v>87.240944</v>
       </c>
       <c r="G63" t="n">
         <v>495200</v>

</xml_diff>

<commit_message>
blk stuff and vg nav
</commit_message>
<xml_diff>
--- a/utils/yahoofinance/EDV_yahoofin_historical_data.xlsx
+++ b/utils/yahoofinance/EDV_yahoofin_historical_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G208"/>
+  <dimension ref="A1:G209"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -539,7 +539,7 @@
         <v>86.989998</v>
       </c>
       <c r="F4" t="n">
-        <v>83.820305</v>
+        <v>83.820297</v>
       </c>
       <c r="G4" t="n">
         <v>383400</v>
@@ -639,7 +639,7 @@
         <v>89.5</v>
       </c>
       <c r="F8" t="n">
-        <v>86.238846</v>
+        <v>86.23885300000001</v>
       </c>
       <c r="G8" t="n">
         <v>158700</v>
@@ -739,7 +739,7 @@
         <v>92.83000199999999</v>
       </c>
       <c r="F12" t="n">
-        <v>89.44750999999999</v>
+        <v>89.447517</v>
       </c>
       <c r="G12" t="n">
         <v>334400</v>
@@ -814,7 +814,7 @@
         <v>89.5</v>
       </c>
       <c r="F15" t="n">
-        <v>86.238846</v>
+        <v>86.23885300000001</v>
       </c>
       <c r="G15" t="n">
         <v>250400</v>
@@ -839,7 +839,7 @@
         <v>91.239998</v>
       </c>
       <c r="F16" t="n">
-        <v>87.915436</v>
+        <v>87.915443</v>
       </c>
       <c r="G16" t="n">
         <v>161100</v>
@@ -1114,7 +1114,7 @@
         <v>89.970001</v>
       </c>
       <c r="F27" t="n">
-        <v>86.69171900000001</v>
+        <v>86.691727</v>
       </c>
       <c r="G27" t="n">
         <v>212600</v>
@@ -1264,7 +1264,7 @@
         <v>85.43000000000001</v>
       </c>
       <c r="F33" t="n">
-        <v>82.317154</v>
+        <v>82.31714599999999</v>
       </c>
       <c r="G33" t="n">
         <v>466900</v>
@@ -1339,7 +1339,7 @@
         <v>85.300003</v>
       </c>
       <c r="F36" t="n">
-        <v>82.191895</v>
+        <v>82.19188699999999</v>
       </c>
       <c r="G36" t="n">
         <v>115300</v>
@@ -1414,7 +1414,7 @@
         <v>85.160004</v>
       </c>
       <c r="F39" t="n">
-        <v>82.056984</v>
+        <v>82.05699199999999</v>
       </c>
       <c r="G39" t="n">
         <v>283500</v>
@@ -1614,7 +1614,7 @@
         <v>86.44000200000001</v>
       </c>
       <c r="F47" t="n">
-        <v>83.290352</v>
+        <v>83.290344</v>
       </c>
       <c r="G47" t="n">
         <v>143000</v>
@@ -1714,7 +1714,7 @@
         <v>90.449997</v>
       </c>
       <c r="F51" t="n">
-        <v>87.154236</v>
+        <v>87.154228</v>
       </c>
       <c r="G51" t="n">
         <v>341500</v>
@@ -1814,7 +1814,7 @@
         <v>89.30999799999999</v>
       </c>
       <c r="F55" t="n">
-        <v>86.055763</v>
+        <v>86.05577099999999</v>
       </c>
       <c r="G55" t="n">
         <v>845800</v>
@@ -1864,7 +1864,7 @@
         <v>89.910004</v>
       </c>
       <c r="F57" t="n">
-        <v>86.633904</v>
+        <v>86.633911</v>
       </c>
       <c r="G57" t="n">
         <v>884900</v>
@@ -1989,7 +1989,7 @@
         <v>88.610001</v>
       </c>
       <c r="F62" t="n">
-        <v>85.381271</v>
+        <v>85.38127900000001</v>
       </c>
       <c r="G62" t="n">
         <v>299600</v>
@@ -2014,7 +2014,7 @@
         <v>90.540001</v>
       </c>
       <c r="F63" t="n">
-        <v>87.240944</v>
+        <v>87.24095199999999</v>
       </c>
       <c r="G63" t="n">
         <v>495200</v>
@@ -5643,6 +5643,31 @@
       </c>
       <c r="G208" t="n">
         <v>709400</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>2023-10-30</t>
+        </is>
+      </c>
+      <c r="B209" t="n">
+        <v>63.880001</v>
+      </c>
+      <c r="C209" t="n">
+        <v>64.519897</v>
+      </c>
+      <c r="D209" t="n">
+        <v>63.224998</v>
+      </c>
+      <c r="E209" t="n">
+        <v>64.120003</v>
+      </c>
+      <c r="F209" t="n">
+        <v>64.120003</v>
+      </c>
+      <c r="G209" t="n">
+        <v>673538</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
daily summary book works for vg
</commit_message>
<xml_diff>
--- a/utils/yahoofinance/EDV_yahoofin_historical_data.xlsx
+++ b/utils/yahoofinance/EDV_yahoofin_historical_data.xlsx
@@ -614,7 +614,7 @@
         <v>87.529999</v>
       </c>
       <c r="F7" t="n">
-        <v>84.340622</v>
+        <v>84.34063</v>
       </c>
       <c r="G7" t="n">
         <v>329500</v>
@@ -639,7 +639,7 @@
         <v>89.5</v>
       </c>
       <c r="F8" t="n">
-        <v>86.23885300000001</v>
+        <v>86.238846</v>
       </c>
       <c r="G8" t="n">
         <v>158700</v>
@@ -689,7 +689,7 @@
         <v>90.949997</v>
       </c>
       <c r="F10" t="n">
-        <v>87.636009</v>
+        <v>87.636017</v>
       </c>
       <c r="G10" t="n">
         <v>290200</v>
@@ -764,7 +764,7 @@
         <v>92.129997</v>
       </c>
       <c r="F13" t="n">
-        <v>88.77301</v>
+        <v>88.77301799999999</v>
       </c>
       <c r="G13" t="n">
         <v>235000</v>
@@ -814,7 +814,7 @@
         <v>89.5</v>
       </c>
       <c r="F15" t="n">
-        <v>86.23885300000001</v>
+        <v>86.238846</v>
       </c>
       <c r="G15" t="n">
         <v>250400</v>
@@ -889,7 +889,7 @@
         <v>91.139999</v>
       </c>
       <c r="F18" t="n">
-        <v>87.819084</v>
+        <v>87.819092</v>
       </c>
       <c r="G18" t="n">
         <v>184000</v>
@@ -964,7 +964,7 @@
         <v>91.260002</v>
       </c>
       <c r="F21" t="n">
-        <v>87.934715</v>
+        <v>87.93472300000001</v>
       </c>
       <c r="G21" t="n">
         <v>228600</v>
@@ -1039,7 +1039,7 @@
         <v>91.41999800000001</v>
       </c>
       <c r="F24" t="n">
-        <v>88.08889000000001</v>
+        <v>88.088882</v>
       </c>
       <c r="G24" t="n">
         <v>353200</v>
@@ -1289,7 +1289,7 @@
         <v>86.300003</v>
       </c>
       <c r="F34" t="n">
-        <v>83.155449</v>
+        <v>83.155457</v>
       </c>
       <c r="G34" t="n">
         <v>164100</v>
@@ -1314,7 +1314,7 @@
         <v>84.129997</v>
       </c>
       <c r="F35" t="n">
-        <v>81.06450700000001</v>
+        <v>81.064514</v>
       </c>
       <c r="G35" t="n">
         <v>356800</v>
@@ -1339,7 +1339,7 @@
         <v>85.300003</v>
       </c>
       <c r="F36" t="n">
-        <v>82.19188699999999</v>
+        <v>82.191879</v>
       </c>
       <c r="G36" t="n">
         <v>115300</v>
@@ -1364,7 +1364,7 @@
         <v>86.480003</v>
       </c>
       <c r="F37" t="n">
-        <v>83.32888800000001</v>
+        <v>83.328896</v>
       </c>
       <c r="G37" t="n">
         <v>138900</v>
@@ -1414,7 +1414,7 @@
         <v>85.160004</v>
       </c>
       <c r="F39" t="n">
-        <v>82.05699199999999</v>
+        <v>82.056984</v>
       </c>
       <c r="G39" t="n">
         <v>283500</v>
@@ -1439,7 +1439,7 @@
         <v>85.449997</v>
       </c>
       <c r="F40" t="n">
-        <v>82.33641799999999</v>
+        <v>82.336411</v>
       </c>
       <c r="G40" t="n">
         <v>157800</v>
@@ -1489,7 +1489,7 @@
         <v>83.610001</v>
       </c>
       <c r="F42" t="n">
-        <v>80.563469</v>
+        <v>80.563461</v>
       </c>
       <c r="G42" t="n">
         <v>237500</v>
@@ -1514,7 +1514,7 @@
         <v>86.400002</v>
       </c>
       <c r="F43" t="n">
-        <v>83.251808</v>
+        <v>83.251801</v>
       </c>
       <c r="G43" t="n">
         <v>185500</v>
@@ -1539,7 +1539,7 @@
         <v>85.519997</v>
       </c>
       <c r="F44" t="n">
-        <v>82.403862</v>
+        <v>82.40387</v>
       </c>
       <c r="G44" t="n">
         <v>169400</v>
@@ -1639,7 +1639,7 @@
         <v>90.269997</v>
       </c>
       <c r="F48" t="n">
-        <v>86.980782</v>
+        <v>86.980789</v>
       </c>
       <c r="G48" t="n">
         <v>657100</v>
@@ -1689,7 +1689,7 @@
         <v>88.300003</v>
       </c>
       <c r="F50" t="n">
-        <v>85.082573</v>
+        <v>85.082581</v>
       </c>
       <c r="G50" t="n">
         <v>444700</v>
@@ -1714,7 +1714,7 @@
         <v>90.449997</v>
       </c>
       <c r="F51" t="n">
-        <v>87.154228</v>
+        <v>87.15422100000001</v>
       </c>
       <c r="G51" t="n">
         <v>341500</v>
@@ -1814,7 +1814,7 @@
         <v>89.30999799999999</v>
       </c>
       <c r="F55" t="n">
-        <v>86.05577099999999</v>
+        <v>86.055763</v>
       </c>
       <c r="G55" t="n">
         <v>845800</v>
@@ -1914,7 +1914,7 @@
         <v>88.150002</v>
       </c>
       <c r="F59" t="n">
-        <v>84.938034</v>
+        <v>84.938042</v>
       </c>
       <c r="G59" t="n">
         <v>1142600</v>
@@ -1939,7 +1939,7 @@
         <v>88.300003</v>
       </c>
       <c r="F60" t="n">
-        <v>85.082573</v>
+        <v>85.082581</v>
       </c>
       <c r="G60" t="n">
         <v>847100</v>
@@ -2314,7 +2314,7 @@
         <v>87.459999</v>
       </c>
       <c r="F75" t="n">
-        <v>84.905235</v>
+        <v>84.90522799999999</v>
       </c>
       <c r="G75" t="n">
         <v>563400</v>
@@ -2514,7 +2514,7 @@
         <v>86.540001</v>
       </c>
       <c r="F83" t="n">
-        <v>84.012108</v>
+        <v>84.0121</v>
       </c>
       <c r="G83" t="n">
         <v>850900</v>
@@ -2614,7 +2614,7 @@
         <v>88.220001</v>
       </c>
       <c r="F87" t="n">
-        <v>85.643036</v>
+        <v>85.643028</v>
       </c>
       <c r="G87" t="n">
         <v>466000</v>
@@ -2664,7 +2664,7 @@
         <v>86.150002</v>
       </c>
       <c r="F89" t="n">
-        <v>83.633499</v>
+        <v>83.633492</v>
       </c>
       <c r="G89" t="n">
         <v>351900</v>
@@ -2689,7 +2689,7 @@
         <v>87.099998</v>
       </c>
       <c r="F90" t="n">
-        <v>84.55574799999999</v>
+        <v>84.55574</v>
       </c>
       <c r="G90" t="n">
         <v>513900</v>
@@ -2739,7 +2739,7 @@
         <v>87.449997</v>
       </c>
       <c r="F92" t="n">
-        <v>84.895515</v>
+        <v>84.895523</v>
       </c>
       <c r="G92" t="n">
         <v>184800</v>
@@ -2764,7 +2764,7 @@
         <v>86.269997</v>
       </c>
       <c r="F93" t="n">
-        <v>83.74999200000001</v>
+        <v>83.749985</v>
       </c>
       <c r="G93" t="n">
         <v>382900</v>
@@ -2889,7 +2889,7 @@
         <v>83.58000199999999</v>
       </c>
       <c r="F98" t="n">
-        <v>81.13857299999999</v>
+        <v>81.138565</v>
       </c>
       <c r="G98" t="n">
         <v>390300</v>
@@ -2914,7 +2914,7 @@
         <v>83.959999</v>
       </c>
       <c r="F99" t="n">
-        <v>81.507462</v>
+        <v>81.507469</v>
       </c>
       <c r="G99" t="n">
         <v>396600</v>
@@ -2964,7 +2964,7 @@
         <v>83.349998</v>
       </c>
       <c r="F101" t="n">
-        <v>80.915283</v>
+        <v>80.915291</v>
       </c>
       <c r="G101" t="n">
         <v>374500</v>
@@ -2989,7 +2989,7 @@
         <v>84.279999</v>
       </c>
       <c r="F102" t="n">
-        <v>81.818123</v>
+        <v>81.81811500000001</v>
       </c>
       <c r="G102" t="n">
         <v>274700</v>
@@ -3164,7 +3164,7 @@
         <v>84.400002</v>
       </c>
       <c r="F109" t="n">
-        <v>81.934624</v>
+        <v>81.93461600000001</v>
       </c>
       <c r="G109" t="n">
         <v>531700</v>
@@ -3289,7 +3289,7 @@
         <v>85.980003</v>
       </c>
       <c r="F114" t="n">
-        <v>83.468468</v>
+        <v>83.46845999999999</v>
       </c>
       <c r="G114" t="n">
         <v>154000</v>
@@ -3364,7 +3364,7 @@
         <v>87.43000000000001</v>
       </c>
       <c r="F117" t="n">
-        <v>84.87610599999999</v>
+        <v>84.876114</v>
       </c>
       <c r="G117" t="n">
         <v>205800</v>
@@ -3539,7 +3539,7 @@
         <v>85.699997</v>
       </c>
       <c r="F124" t="n">
-        <v>83.19664</v>
+        <v>83.19663199999999</v>
       </c>
       <c r="G124" t="n">
         <v>342900</v>
@@ -3564,7 +3564,7 @@
         <v>87.06999999999999</v>
       </c>
       <c r="F125" t="n">
-        <v>84.526627</v>
+        <v>84.526619</v>
       </c>
       <c r="G125" t="n">
         <v>190000</v>
@@ -5655,10 +5655,10 @@
         <v>63.880001</v>
       </c>
       <c r="C209" t="n">
-        <v>64.519897</v>
+        <v>64.519997</v>
       </c>
       <c r="D209" t="n">
-        <v>63.224998</v>
+        <v>63.18</v>
       </c>
       <c r="E209" t="n">
         <v>64.120003</v>
@@ -5667,7 +5667,7 @@
         <v>64.120003</v>
       </c>
       <c r="G209" t="n">
-        <v>673538</v>
+        <v>673500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
vg fund risk metrics
</commit_message>
<xml_diff>
--- a/utils/yahoofinance/EDV_yahoofin_historical_data.xlsx
+++ b/utils/yahoofinance/EDV_yahoofin_historical_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G209"/>
+  <dimension ref="A1:G214"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -614,7 +614,7 @@
         <v>87.529999</v>
       </c>
       <c r="F7" t="n">
-        <v>84.34063</v>
+        <v>84.340622</v>
       </c>
       <c r="G7" t="n">
         <v>329500</v>
@@ -639,7 +639,7 @@
         <v>89.5</v>
       </c>
       <c r="F8" t="n">
-        <v>86.238846</v>
+        <v>86.238838</v>
       </c>
       <c r="G8" t="n">
         <v>158700</v>
@@ -689,7 +689,7 @@
         <v>90.949997</v>
       </c>
       <c r="F10" t="n">
-        <v>87.636017</v>
+        <v>87.636009</v>
       </c>
       <c r="G10" t="n">
         <v>290200</v>
@@ -739,7 +739,7 @@
         <v>92.83000199999999</v>
       </c>
       <c r="F12" t="n">
-        <v>89.447517</v>
+        <v>89.44750999999999</v>
       </c>
       <c r="G12" t="n">
         <v>334400</v>
@@ -764,7 +764,7 @@
         <v>92.129997</v>
       </c>
       <c r="F13" t="n">
-        <v>88.77301799999999</v>
+        <v>88.77301</v>
       </c>
       <c r="G13" t="n">
         <v>235000</v>
@@ -814,7 +814,7 @@
         <v>89.5</v>
       </c>
       <c r="F15" t="n">
-        <v>86.238846</v>
+        <v>86.238838</v>
       </c>
       <c r="G15" t="n">
         <v>250400</v>
@@ -864,7 +864,7 @@
         <v>91.55999799999999</v>
       </c>
       <c r="F17" t="n">
-        <v>88.223778</v>
+        <v>88.22378500000001</v>
       </c>
       <c r="G17" t="n">
         <v>141400</v>
@@ -914,7 +914,7 @@
         <v>90.980003</v>
       </c>
       <c r="F19" t="n">
-        <v>87.664925</v>
+        <v>87.664917</v>
       </c>
       <c r="G19" t="n">
         <v>220800</v>
@@ -964,7 +964,7 @@
         <v>91.260002</v>
       </c>
       <c r="F21" t="n">
-        <v>87.93472300000001</v>
+        <v>87.934715</v>
       </c>
       <c r="G21" t="n">
         <v>228600</v>
@@ -989,7 +989,7 @@
         <v>92.91999800000001</v>
       </c>
       <c r="F22" t="n">
-        <v>89.53422500000001</v>
+        <v>89.534233</v>
       </c>
       <c r="G22" t="n">
         <v>426700</v>
@@ -1039,7 +1039,7 @@
         <v>91.41999800000001</v>
       </c>
       <c r="F24" t="n">
-        <v>88.088882</v>
+        <v>88.08889000000001</v>
       </c>
       <c r="G24" t="n">
         <v>353200</v>
@@ -1139,7 +1139,7 @@
         <v>88.839996</v>
       </c>
       <c r="F28" t="n">
-        <v>85.60289</v>
+        <v>85.602898</v>
       </c>
       <c r="G28" t="n">
         <v>265600</v>
@@ -1289,7 +1289,7 @@
         <v>86.300003</v>
       </c>
       <c r="F34" t="n">
-        <v>83.155457</v>
+        <v>83.155449</v>
       </c>
       <c r="G34" t="n">
         <v>164100</v>
@@ -1339,7 +1339,7 @@
         <v>85.300003</v>
       </c>
       <c r="F36" t="n">
-        <v>82.191879</v>
+        <v>82.19188699999999</v>
       </c>
       <c r="G36" t="n">
         <v>115300</v>
@@ -1539,7 +1539,7 @@
         <v>85.519997</v>
       </c>
       <c r="F44" t="n">
-        <v>82.40387</v>
+        <v>82.403862</v>
       </c>
       <c r="G44" t="n">
         <v>169400</v>
@@ -1564,7 +1564,7 @@
         <v>86.260002</v>
       </c>
       <c r="F45" t="n">
-        <v>83.116905</v>
+        <v>83.11689800000001</v>
       </c>
       <c r="G45" t="n">
         <v>138900</v>
@@ -1614,7 +1614,7 @@
         <v>86.44000200000001</v>
       </c>
       <c r="F47" t="n">
-        <v>83.290344</v>
+        <v>83.290352</v>
       </c>
       <c r="G47" t="n">
         <v>143000</v>
@@ -1689,7 +1689,7 @@
         <v>88.300003</v>
       </c>
       <c r="F50" t="n">
-        <v>85.082581</v>
+        <v>85.082573</v>
       </c>
       <c r="G50" t="n">
         <v>444700</v>
@@ -1714,7 +1714,7 @@
         <v>90.449997</v>
       </c>
       <c r="F51" t="n">
-        <v>87.15422100000001</v>
+        <v>87.154228</v>
       </c>
       <c r="G51" t="n">
         <v>341500</v>
@@ -1764,7 +1764,7 @@
         <v>91.31999999999999</v>
       </c>
       <c r="F53" t="n">
-        <v>87.992531</v>
+        <v>87.99252300000001</v>
       </c>
       <c r="G53" t="n">
         <v>418500</v>
@@ -1789,7 +1789,7 @@
         <v>90.110001</v>
       </c>
       <c r="F54" t="n">
-        <v>86.826622</v>
+        <v>86.82662999999999</v>
       </c>
       <c r="G54" t="n">
         <v>350000</v>
@@ -1939,7 +1939,7 @@
         <v>88.300003</v>
       </c>
       <c r="F60" t="n">
-        <v>85.082581</v>
+        <v>85.082573</v>
       </c>
       <c r="G60" t="n">
         <v>847100</v>
@@ -1989,7 +1989,7 @@
         <v>88.610001</v>
       </c>
       <c r="F62" t="n">
-        <v>85.38127900000001</v>
+        <v>85.381271</v>
       </c>
       <c r="G62" t="n">
         <v>299600</v>
@@ -5668,6 +5668,131 @@
       </c>
       <c r="G209" t="n">
         <v>673500</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>2023-10-31</t>
+        </is>
+      </c>
+      <c r="B210" t="n">
+        <v>64.519997</v>
+      </c>
+      <c r="C210" t="n">
+        <v>64.970001</v>
+      </c>
+      <c r="D210" t="n">
+        <v>63.549999</v>
+      </c>
+      <c r="E210" t="n">
+        <v>63.740002</v>
+      </c>
+      <c r="F210" t="n">
+        <v>63.740002</v>
+      </c>
+      <c r="G210" t="n">
+        <v>501700</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>2023-11-01</t>
+        </is>
+      </c>
+      <c r="B211" t="n">
+        <v>64.400002</v>
+      </c>
+      <c r="C211" t="n">
+        <v>65.620003</v>
+      </c>
+      <c r="D211" t="n">
+        <v>64.400002</v>
+      </c>
+      <c r="E211" t="n">
+        <v>65.41999800000001</v>
+      </c>
+      <c r="F211" t="n">
+        <v>65.41999800000001</v>
+      </c>
+      <c r="G211" t="n">
+        <v>611400</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>2023-11-02</t>
+        </is>
+      </c>
+      <c r="B212" t="n">
+        <v>67.33000199999999</v>
+      </c>
+      <c r="C212" t="n">
+        <v>68.120003</v>
+      </c>
+      <c r="D212" t="n">
+        <v>66.870003</v>
+      </c>
+      <c r="E212" t="n">
+        <v>67.800003</v>
+      </c>
+      <c r="F212" t="n">
+        <v>67.800003</v>
+      </c>
+      <c r="G212" t="n">
+        <v>737200</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>2023-11-03</t>
+        </is>
+      </c>
+      <c r="B213" t="n">
+        <v>69.81999999999999</v>
+      </c>
+      <c r="C213" t="n">
+        <v>69.959999</v>
+      </c>
+      <c r="D213" t="n">
+        <v>68.300003</v>
+      </c>
+      <c r="E213" t="n">
+        <v>68.370003</v>
+      </c>
+      <c r="F213" t="n">
+        <v>68.370003</v>
+      </c>
+      <c r="G213" t="n">
+        <v>821900</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>2023-11-06</t>
+        </is>
+      </c>
+      <c r="B214" t="n">
+        <v>67.800003</v>
+      </c>
+      <c r="C214" t="n">
+        <v>67.94000200000001</v>
+      </c>
+      <c r="D214" t="n">
+        <v>67.290001</v>
+      </c>
+      <c r="E214" t="n">
+        <v>67.519997</v>
+      </c>
+      <c r="F214" t="n">
+        <v>67.519997</v>
+      </c>
+      <c r="G214" t="n">
+        <v>500742</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cool yield curve graphs
</commit_message>
<xml_diff>
--- a/utils/yahoofinance/EDV_yahoofin_historical_data.xlsx
+++ b/utils/yahoofinance/EDV_yahoofin_historical_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G215"/>
+  <dimension ref="A1:G216"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -614,7 +614,7 @@
         <v>87.529999</v>
       </c>
       <c r="F7" t="n">
-        <v>84.34063</v>
+        <v>84.340622</v>
       </c>
       <c r="G7" t="n">
         <v>329500</v>
@@ -639,7 +639,7 @@
         <v>89.5</v>
       </c>
       <c r="F8" t="n">
-        <v>86.238846</v>
+        <v>86.238838</v>
       </c>
       <c r="G8" t="n">
         <v>158700</v>
@@ -689,7 +689,7 @@
         <v>90.949997</v>
       </c>
       <c r="F10" t="n">
-        <v>87.636017</v>
+        <v>87.636009</v>
       </c>
       <c r="G10" t="n">
         <v>290200</v>
@@ -739,7 +739,7 @@
         <v>92.83000199999999</v>
       </c>
       <c r="F12" t="n">
-        <v>89.447517</v>
+        <v>89.44750999999999</v>
       </c>
       <c r="G12" t="n">
         <v>334400</v>
@@ -764,7 +764,7 @@
         <v>92.129997</v>
       </c>
       <c r="F13" t="n">
-        <v>88.77301799999999</v>
+        <v>88.77301</v>
       </c>
       <c r="G13" t="n">
         <v>235000</v>
@@ -814,7 +814,7 @@
         <v>89.5</v>
       </c>
       <c r="F15" t="n">
-        <v>86.238846</v>
+        <v>86.238838</v>
       </c>
       <c r="G15" t="n">
         <v>250400</v>
@@ -864,7 +864,7 @@
         <v>91.55999799999999</v>
       </c>
       <c r="F17" t="n">
-        <v>88.223778</v>
+        <v>88.22378500000001</v>
       </c>
       <c r="G17" t="n">
         <v>141400</v>
@@ -914,7 +914,7 @@
         <v>90.980003</v>
       </c>
       <c r="F19" t="n">
-        <v>87.664925</v>
+        <v>87.664917</v>
       </c>
       <c r="G19" t="n">
         <v>220800</v>
@@ -964,7 +964,7 @@
         <v>91.260002</v>
       </c>
       <c r="F21" t="n">
-        <v>87.93472300000001</v>
+        <v>87.934715</v>
       </c>
       <c r="G21" t="n">
         <v>228600</v>
@@ -989,7 +989,7 @@
         <v>92.91999800000001</v>
       </c>
       <c r="F22" t="n">
-        <v>89.53422500000001</v>
+        <v>89.534233</v>
       </c>
       <c r="G22" t="n">
         <v>426700</v>
@@ -1039,7 +1039,7 @@
         <v>91.41999800000001</v>
       </c>
       <c r="F24" t="n">
-        <v>88.088882</v>
+        <v>88.08889000000001</v>
       </c>
       <c r="G24" t="n">
         <v>353200</v>
@@ -1139,7 +1139,7 @@
         <v>88.839996</v>
       </c>
       <c r="F28" t="n">
-        <v>85.60289</v>
+        <v>85.602898</v>
       </c>
       <c r="G28" t="n">
         <v>265600</v>
@@ -1289,7 +1289,7 @@
         <v>86.300003</v>
       </c>
       <c r="F34" t="n">
-        <v>83.155457</v>
+        <v>83.155449</v>
       </c>
       <c r="G34" t="n">
         <v>164100</v>
@@ -1339,7 +1339,7 @@
         <v>85.300003</v>
       </c>
       <c r="F36" t="n">
-        <v>82.191879</v>
+        <v>82.19188699999999</v>
       </c>
       <c r="G36" t="n">
         <v>115300</v>
@@ -1539,7 +1539,7 @@
         <v>85.519997</v>
       </c>
       <c r="F44" t="n">
-        <v>82.40387</v>
+        <v>82.403862</v>
       </c>
       <c r="G44" t="n">
         <v>169400</v>
@@ -1564,7 +1564,7 @@
         <v>86.260002</v>
       </c>
       <c r="F45" t="n">
-        <v>83.116905</v>
+        <v>83.11689800000001</v>
       </c>
       <c r="G45" t="n">
         <v>138900</v>
@@ -1614,7 +1614,7 @@
         <v>86.44000200000001</v>
       </c>
       <c r="F47" t="n">
-        <v>83.290344</v>
+        <v>83.290352</v>
       </c>
       <c r="G47" t="n">
         <v>143000</v>
@@ -1689,7 +1689,7 @@
         <v>88.300003</v>
       </c>
       <c r="F50" t="n">
-        <v>85.082581</v>
+        <v>85.082573</v>
       </c>
       <c r="G50" t="n">
         <v>444700</v>
@@ -1714,7 +1714,7 @@
         <v>90.449997</v>
       </c>
       <c r="F51" t="n">
-        <v>87.15422100000001</v>
+        <v>87.154228</v>
       </c>
       <c r="G51" t="n">
         <v>341500</v>
@@ -1764,7 +1764,7 @@
         <v>91.31999999999999</v>
       </c>
       <c r="F53" t="n">
-        <v>87.992531</v>
+        <v>87.99252300000001</v>
       </c>
       <c r="G53" t="n">
         <v>418500</v>
@@ -1789,7 +1789,7 @@
         <v>90.110001</v>
       </c>
       <c r="F54" t="n">
-        <v>86.826622</v>
+        <v>86.82662999999999</v>
       </c>
       <c r="G54" t="n">
         <v>350000</v>
@@ -1939,7 +1939,7 @@
         <v>88.300003</v>
       </c>
       <c r="F60" t="n">
-        <v>85.082581</v>
+        <v>85.082573</v>
       </c>
       <c r="G60" t="n">
         <v>847100</v>
@@ -1989,7 +1989,7 @@
         <v>88.610001</v>
       </c>
       <c r="F62" t="n">
-        <v>85.38127900000001</v>
+        <v>85.381271</v>
       </c>
       <c r="G62" t="n">
         <v>299600</v>
@@ -5805,19 +5805,44 @@
         <v>68.379997</v>
       </c>
       <c r="C215" t="n">
-        <v>69.06999999999999</v>
+        <v>69.400002</v>
       </c>
       <c r="D215" t="n">
-        <v>68.394997</v>
+        <v>68.379997</v>
       </c>
       <c r="E215" t="n">
-        <v>69.06999999999999</v>
+        <v>68.839996</v>
       </c>
       <c r="F215" t="n">
-        <v>69.06999999999999</v>
+        <v>68.839996</v>
       </c>
       <c r="G215" t="n">
-        <v>297818</v>
+        <v>454800</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>2023-11-08</t>
+        </is>
+      </c>
+      <c r="B216" t="n">
+        <v>69.389999</v>
+      </c>
+      <c r="C216" t="n">
+        <v>70.720001</v>
+      </c>
+      <c r="D216" t="n">
+        <v>69.339996</v>
+      </c>
+      <c r="E216" t="n">
+        <v>70.650002</v>
+      </c>
+      <c r="F216" t="n">
+        <v>70.650002</v>
+      </c>
+      <c r="G216" t="n">
+        <v>472692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>